<commit_message>
The merged and updated table
</commit_message>
<xml_diff>
--- a/data_final.xlsx
+++ b/data_final.xlsx
@@ -739,7 +739,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -754,6 +754,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1282,8 +1285,8 @@
   <sheetPr/>
   <dimension ref="A1:T608"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A585" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A481" workbookViewId="0">
+      <selection activeCell="A381" sqref="A381:A608"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.02654867256637" defaultRowHeight="13.5"/>
@@ -12267,7 +12270,7 @@
       </c>
     </row>
     <row r="381" spans="1:7">
-      <c r="A381" t="s">
+      <c r="A381" s="5" t="s">
         <v>26</v>
       </c>
       <c r="B381" s="1" t="s">
@@ -12289,7 +12292,8 @@
         <v>29</v>
       </c>
     </row>
-    <row r="382" spans="2:7">
+    <row r="382" spans="1:7">
+      <c r="A382" s="5"/>
       <c r="B382" s="1"/>
       <c r="C382" s="2">
         <v>1</v>
@@ -12307,7 +12311,8 @@
         <v>0.428571428571429</v>
       </c>
     </row>
-    <row r="383" spans="2:7">
+    <row r="383" spans="1:7">
+      <c r="A383" s="5"/>
       <c r="B383" s="1"/>
       <c r="C383" s="2">
         <v>2</v>
@@ -12325,7 +12330,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="384" spans="2:7">
+    <row r="384" spans="1:7">
+      <c r="A384" s="5"/>
       <c r="B384" s="1"/>
       <c r="C384" s="2">
         <v>3</v>
@@ -12343,7 +12349,8 @@
         <v>0.428571428571429</v>
       </c>
     </row>
-    <row r="385" spans="2:7">
+    <row r="385" spans="1:7">
+      <c r="A385" s="5"/>
       <c r="B385" s="1"/>
       <c r="C385" s="2">
         <v>4</v>
@@ -12361,7 +12368,8 @@
         <v>0.428571428571429</v>
       </c>
     </row>
-    <row r="386" spans="2:7">
+    <row r="386" spans="1:7">
+      <c r="A386" s="5"/>
       <c r="B386" s="1"/>
       <c r="C386" s="2">
         <v>5</v>
@@ -12379,7 +12387,8 @@
         <v>0.428571428571429</v>
       </c>
     </row>
-    <row r="387" spans="2:7">
+    <row r="387" spans="1:7">
+      <c r="A387" s="5"/>
       <c r="B387" s="1"/>
       <c r="C387" s="2">
         <v>6</v>
@@ -12397,7 +12406,8 @@
         <v>0.928571428571429</v>
       </c>
     </row>
-    <row r="388" spans="2:7">
+    <row r="388" spans="1:7">
+      <c r="A388" s="5"/>
       <c r="B388" s="1"/>
       <c r="C388" s="2">
         <v>7</v>
@@ -12415,7 +12425,8 @@
         <v>0.428571428571429</v>
       </c>
     </row>
-    <row r="389" spans="2:7">
+    <row r="389" spans="1:7">
+      <c r="A389" s="5"/>
       <c r="B389" s="1"/>
       <c r="C389" s="2">
         <v>8</v>
@@ -12433,7 +12444,8 @@
         <v>0.428571428571429</v>
       </c>
     </row>
-    <row r="390" spans="2:7">
+    <row r="390" spans="1:7">
+      <c r="A390" s="5"/>
       <c r="B390" s="1"/>
       <c r="C390" s="2">
         <v>9</v>
@@ -12451,7 +12463,8 @@
         <v>0.785714285714286</v>
       </c>
     </row>
-    <row r="391" spans="2:7">
+    <row r="391" spans="1:7">
+      <c r="A391" s="5"/>
       <c r="B391" s="1"/>
       <c r="C391" s="2">
         <v>10</v>
@@ -12469,7 +12482,8 @@
         <v>0.785714285714286</v>
       </c>
     </row>
-    <row r="392" spans="2:7">
+    <row r="392" spans="1:7">
+      <c r="A392" s="5"/>
       <c r="B392" s="1"/>
       <c r="C392" s="2">
         <v>11</v>
@@ -12487,7 +12501,8 @@
         <v>0.857142857142857</v>
       </c>
     </row>
-    <row r="393" spans="2:7">
+    <row r="393" spans="1:7">
+      <c r="A393" s="5"/>
       <c r="B393" s="1"/>
       <c r="C393" s="2">
         <v>12</v>
@@ -12505,7 +12520,8 @@
         <v>0.428571428571429</v>
       </c>
     </row>
-    <row r="394" spans="2:7">
+    <row r="394" spans="1:7">
+      <c r="A394" s="5"/>
       <c r="B394" s="1"/>
       <c r="C394" s="2">
         <v>13</v>
@@ -12523,7 +12539,8 @@
         <v>0.428571428571429</v>
       </c>
     </row>
-    <row r="395" spans="2:7">
+    <row r="395" spans="1:7">
+      <c r="A395" s="5"/>
       <c r="B395" s="1"/>
       <c r="C395" s="2">
         <v>14</v>
@@ -12541,7 +12558,8 @@
         <v>0.428571428571429</v>
       </c>
     </row>
-    <row r="396" spans="2:7">
+    <row r="396" spans="1:7">
+      <c r="A396" s="5"/>
       <c r="B396" s="1"/>
       <c r="C396" s="2">
         <v>15</v>
@@ -12559,7 +12577,8 @@
         <v>0.428571428571429</v>
       </c>
     </row>
-    <row r="397" spans="2:7">
+    <row r="397" spans="1:7">
+      <c r="A397" s="5"/>
       <c r="B397" s="1"/>
       <c r="C397" s="2">
         <v>16</v>
@@ -12577,7 +12596,8 @@
         <v>0.428571428571429</v>
       </c>
     </row>
-    <row r="398" spans="2:7">
+    <row r="398" spans="1:7">
+      <c r="A398" s="5"/>
       <c r="B398" s="1"/>
       <c r="C398" s="2">
         <v>17</v>
@@ -12595,7 +12615,8 @@
         <v>0.785714285714286</v>
       </c>
     </row>
-    <row r="399" spans="2:7">
+    <row r="399" spans="1:7">
+      <c r="A399" s="5"/>
       <c r="B399" s="1"/>
       <c r="C399" s="2">
         <v>18</v>
@@ -12613,7 +12634,8 @@
         <v>0.428571428571429</v>
       </c>
     </row>
-    <row r="400" spans="2:7">
+    <row r="400" spans="1:7">
+      <c r="A400" s="5"/>
       <c r="B400" s="1"/>
       <c r="C400" s="2">
         <v>19</v>
@@ -12631,7 +12653,8 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="401" spans="2:7">
+    <row r="401" spans="1:7">
+      <c r="A401" s="5"/>
       <c r="B401" s="1"/>
       <c r="C401" s="2">
         <v>20</v>
@@ -12649,7 +12672,8 @@
         <v>0.785714285714286</v>
       </c>
     </row>
-    <row r="402" spans="2:7">
+    <row r="402" spans="1:7">
+      <c r="A402" s="5"/>
       <c r="B402" s="1"/>
       <c r="C402" s="2">
         <v>21</v>
@@ -12667,7 +12691,8 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="403" spans="2:7">
+    <row r="403" spans="1:7">
+      <c r="A403" s="5"/>
       <c r="B403" s="1"/>
       <c r="C403" s="2">
         <v>22</v>
@@ -12685,7 +12710,8 @@
         <v>0.357142857142857</v>
       </c>
     </row>
-    <row r="404" spans="2:7">
+    <row r="404" spans="1:7">
+      <c r="A404" s="5"/>
       <c r="B404" s="1"/>
       <c r="C404" s="2">
         <v>23</v>
@@ -12703,7 +12729,8 @@
         <v>0.785714285714286</v>
       </c>
     </row>
-    <row r="405" spans="2:7">
+    <row r="405" spans="1:7">
+      <c r="A405" s="5"/>
       <c r="B405" s="1"/>
       <c r="C405" s="2">
         <v>24</v>
@@ -12721,7 +12748,8 @@
         <v>0.785714285714286</v>
       </c>
     </row>
-    <row r="406" spans="2:7">
+    <row r="406" spans="1:7">
+      <c r="A406" s="5"/>
       <c r="B406" s="1"/>
       <c r="C406" s="2">
         <v>25</v>
@@ -12739,7 +12767,8 @@
         <v>0.428571428571429</v>
       </c>
     </row>
-    <row r="407" spans="2:7">
+    <row r="407" spans="1:7">
+      <c r="A407" s="5"/>
       <c r="B407" s="1"/>
       <c r="C407" s="2">
         <v>26</v>
@@ -12757,7 +12786,8 @@
         <v>0.357142857142857</v>
       </c>
     </row>
-    <row r="408" spans="2:7">
+    <row r="408" spans="1:7">
+      <c r="A408" s="5"/>
       <c r="B408" s="1"/>
       <c r="C408" s="2">
         <v>27</v>
@@ -12775,7 +12805,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="409" spans="2:7">
+    <row r="409" spans="1:7">
+      <c r="A409" s="5"/>
       <c r="B409" s="1"/>
       <c r="C409" s="2">
         <v>28</v>
@@ -12793,7 +12824,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="410" spans="2:7">
+    <row r="410" spans="1:7">
+      <c r="A410" s="5"/>
       <c r="B410" s="1"/>
       <c r="C410" s="2">
         <v>29</v>
@@ -12811,7 +12843,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="411" spans="2:7">
+    <row r="411" spans="1:7">
+      <c r="A411" s="5"/>
       <c r="B411" s="1"/>
       <c r="C411" s="2">
         <v>30</v>
@@ -12829,7 +12862,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="412" spans="2:7">
+    <row r="412" spans="1:7">
+      <c r="A412" s="5"/>
       <c r="B412" s="1"/>
       <c r="C412" s="2">
         <v>31</v>
@@ -12847,7 +12881,8 @@
         <v>0.428571428571429</v>
       </c>
     </row>
-    <row r="413" spans="2:7">
+    <row r="413" spans="1:7">
+      <c r="A413" s="5"/>
       <c r="B413" s="1"/>
       <c r="C413" s="2">
         <v>32</v>
@@ -12865,7 +12900,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="414" spans="2:7">
+    <row r="414" spans="1:7">
+      <c r="A414" s="5"/>
       <c r="B414" s="1"/>
       <c r="C414" s="2">
         <v>33</v>
@@ -12883,7 +12919,8 @@
         <v>0.928571428571429</v>
       </c>
     </row>
-    <row r="415" spans="2:7">
+    <row r="415" spans="1:7">
+      <c r="A415" s="5"/>
       <c r="B415" s="1"/>
       <c r="C415" s="2">
         <v>34</v>
@@ -12901,7 +12938,8 @@
         <v>0.785714285714286</v>
       </c>
     </row>
-    <row r="416" spans="2:7">
+    <row r="416" spans="1:7">
+      <c r="A416" s="5"/>
       <c r="B416" s="1"/>
       <c r="C416" s="2">
         <v>35</v>
@@ -12919,7 +12957,8 @@
         <v>0.928571428571429</v>
       </c>
     </row>
-    <row r="417" spans="2:7">
+    <row r="417" spans="1:7">
+      <c r="A417" s="5"/>
       <c r="B417" s="1"/>
       <c r="C417" s="2">
         <v>36</v>
@@ -12937,7 +12976,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="418" spans="2:7">
+    <row r="418" spans="1:7">
+      <c r="A418" s="5"/>
       <c r="B418" s="1"/>
       <c r="C418" s="2">
         <v>37</v>
@@ -12955,7 +12995,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="419" spans="2:7">
+    <row r="419" spans="1:7">
+      <c r="A419" s="5"/>
       <c r="B419" s="1"/>
       <c r="C419" s="2">
         <v>38</v>
@@ -12973,7 +13014,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="420" spans="2:7">
+    <row r="420" spans="1:7">
+      <c r="A420" s="5"/>
       <c r="B420" s="1"/>
       <c r="C420" s="2">
         <v>39</v>
@@ -12991,7 +13033,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="421" spans="2:7">
+    <row r="421" spans="1:7">
+      <c r="A421" s="5"/>
       <c r="B421" s="1"/>
       <c r="C421" s="2">
         <v>40</v>
@@ -13009,7 +13052,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="422" spans="2:7">
+    <row r="422" spans="1:7">
+      <c r="A422" s="5"/>
       <c r="B422" s="1"/>
       <c r="C422" s="2">
         <v>41</v>
@@ -13027,7 +13071,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="423" spans="2:7">
+    <row r="423" spans="1:7">
+      <c r="A423" s="5"/>
       <c r="B423" s="1"/>
       <c r="C423" s="2">
         <v>42</v>
@@ -13045,7 +13090,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="424" spans="2:7">
+    <row r="424" spans="1:7">
+      <c r="A424" s="5"/>
       <c r="B424" s="1"/>
       <c r="C424" s="2">
         <v>43</v>
@@ -13063,7 +13109,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="425" spans="2:7">
+    <row r="425" spans="1:7">
+      <c r="A425" s="5"/>
       <c r="B425" s="1"/>
       <c r="C425" s="2">
         <v>44</v>
@@ -13081,7 +13128,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="426" spans="2:7">
+    <row r="426" spans="1:7">
+      <c r="A426" s="5"/>
       <c r="B426" s="1"/>
       <c r="C426" s="2">
         <v>45</v>
@@ -13099,7 +13147,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="427" spans="2:7">
+    <row r="427" spans="1:7">
+      <c r="A427" s="5"/>
       <c r="B427" s="1"/>
       <c r="C427" s="2">
         <v>46</v>
@@ -13117,7 +13166,8 @@
         <v>0.928571428571429</v>
       </c>
     </row>
-    <row r="428" spans="2:7">
+    <row r="428" spans="1:7">
+      <c r="A428" s="5"/>
       <c r="B428" s="1"/>
       <c r="C428" s="2">
         <v>47</v>
@@ -13135,7 +13185,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="429" spans="2:7">
+    <row r="429" spans="1:7">
+      <c r="A429" s="5"/>
       <c r="B429" s="1"/>
       <c r="C429" s="2">
         <v>48</v>
@@ -13153,7 +13204,8 @@
         <v>0.928571428571429</v>
       </c>
     </row>
-    <row r="430" spans="2:7">
+    <row r="430" spans="1:7">
+      <c r="A430" s="5"/>
       <c r="B430" s="1"/>
       <c r="C430" s="2">
         <v>49</v>
@@ -13171,7 +13223,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="431" spans="2:7">
+    <row r="431" spans="1:7">
+      <c r="A431" s="5"/>
       <c r="B431" s="1"/>
       <c r="C431" s="2">
         <v>50</v>
@@ -13189,7 +13242,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="432" spans="2:7">
+    <row r="432" spans="1:7">
+      <c r="A432" s="5"/>
       <c r="B432" s="1"/>
       <c r="C432" s="2">
         <v>51</v>
@@ -13207,7 +13261,8 @@
         <v>0.714285714285714</v>
       </c>
     </row>
-    <row r="433" spans="2:7">
+    <row r="433" spans="1:7">
+      <c r="A433" s="5"/>
       <c r="B433" s="1"/>
       <c r="C433" s="2">
         <v>52</v>
@@ -13225,7 +13280,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="434" spans="2:7">
+    <row r="434" spans="1:7">
+      <c r="A434" s="5"/>
       <c r="B434" s="1"/>
       <c r="C434" s="2">
         <v>53</v>
@@ -13243,7 +13299,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="435" spans="2:7">
+    <row r="435" spans="1:7">
+      <c r="A435" s="5"/>
       <c r="B435" s="1"/>
       <c r="C435" s="2">
         <v>54</v>
@@ -13261,7 +13318,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="436" spans="2:7">
+    <row r="436" spans="1:7">
+      <c r="A436" s="5"/>
       <c r="B436" s="1"/>
       <c r="C436" s="2">
         <v>55</v>
@@ -13279,7 +13337,8 @@
         <v>0.428571428571429</v>
       </c>
     </row>
-    <row r="437" spans="2:7">
+    <row r="437" spans="1:7">
+      <c r="A437" s="5"/>
       <c r="B437" s="1"/>
       <c r="C437" s="2">
         <v>56</v>
@@ -13297,7 +13356,8 @@
         <v>0.428571428571429</v>
       </c>
     </row>
-    <row r="438" spans="2:7">
+    <row r="438" spans="1:7">
+      <c r="A438" s="5"/>
       <c r="B438" s="1"/>
       <c r="C438" s="2">
         <v>57</v>
@@ -13315,7 +13375,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="439" spans="2:7">
+    <row r="439" spans="1:7">
+      <c r="A439" s="5"/>
       <c r="B439" s="1"/>
       <c r="C439" s="2">
         <v>58</v>
@@ -13333,7 +13394,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="440" spans="2:7">
+    <row r="440" spans="1:7">
+      <c r="A440" s="5"/>
       <c r="B440" s="1"/>
       <c r="C440" s="2">
         <v>59</v>
@@ -13351,7 +13413,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="441" spans="2:7">
+    <row r="441" spans="1:7">
+      <c r="A441" s="5"/>
       <c r="B441" s="1"/>
       <c r="C441" s="2">
         <v>60</v>
@@ -13369,7 +13432,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="442" spans="2:7">
+    <row r="442" spans="1:7">
+      <c r="A442" s="5"/>
       <c r="B442" s="1"/>
       <c r="C442" s="2">
         <v>61</v>
@@ -13387,7 +13451,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="443" spans="2:7">
+    <row r="443" spans="1:7">
+      <c r="A443" s="5"/>
       <c r="B443" s="1"/>
       <c r="C443" s="2">
         <v>62</v>
@@ -13405,7 +13470,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="444" spans="2:7">
+    <row r="444" spans="1:7">
+      <c r="A444" s="5"/>
       <c r="B444" s="1"/>
       <c r="C444" s="2">
         <v>63</v>
@@ -13423,7 +13489,8 @@
         <v>0.428571428571429</v>
       </c>
     </row>
-    <row r="445" spans="2:7">
+    <row r="445" spans="1:7">
+      <c r="A445" s="5"/>
       <c r="B445" s="1"/>
       <c r="C445" s="2">
         <v>64</v>
@@ -13441,7 +13508,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="446" spans="2:7">
+    <row r="446" spans="1:7">
+      <c r="A446" s="5"/>
       <c r="B446" s="1"/>
       <c r="C446" s="2">
         <v>65</v>
@@ -13459,7 +13527,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="447" spans="2:7">
+    <row r="447" spans="1:7">
+      <c r="A447" s="5"/>
       <c r="B447" s="1"/>
       <c r="C447" s="2">
         <v>66</v>
@@ -13477,7 +13546,8 @@
         <v>0.428571428571429</v>
       </c>
     </row>
-    <row r="448" spans="2:7">
+    <row r="448" spans="1:7">
+      <c r="A448" s="5"/>
       <c r="B448" s="1"/>
       <c r="C448" s="2">
         <v>67</v>
@@ -13495,7 +13565,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="449" spans="2:7">
+    <row r="449" spans="1:7">
+      <c r="A449" s="5"/>
       <c r="B449" s="1"/>
       <c r="C449" s="2">
         <v>68</v>
@@ -13513,7 +13584,8 @@
         <v>0.428571428571429</v>
       </c>
     </row>
-    <row r="450" spans="2:7">
+    <row r="450" spans="1:7">
+      <c r="A450" s="5"/>
       <c r="B450" s="1"/>
       <c r="C450" s="2">
         <v>69</v>
@@ -13531,7 +13603,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="451" spans="2:7">
+    <row r="451" spans="1:7">
+      <c r="A451" s="5"/>
       <c r="B451" s="1"/>
       <c r="C451" s="2">
         <v>70</v>
@@ -13549,7 +13622,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="452" spans="2:7">
+    <row r="452" spans="1:7">
+      <c r="A452" s="5"/>
       <c r="B452" s="1"/>
       <c r="C452" s="2">
         <v>71</v>
@@ -13567,7 +13641,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="453" spans="2:7">
+    <row r="453" spans="1:7">
+      <c r="A453" s="5"/>
       <c r="B453" s="1"/>
       <c r="C453" s="2">
         <v>72</v>
@@ -13585,7 +13660,8 @@
         <v>0.428571428571429</v>
       </c>
     </row>
-    <row r="454" spans="2:7">
+    <row r="454" spans="1:7">
+      <c r="A454" s="5"/>
       <c r="B454" s="1"/>
       <c r="C454" s="2">
         <v>73</v>
@@ -13603,7 +13679,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="455" spans="2:7">
+    <row r="455" spans="1:7">
+      <c r="A455" s="5"/>
       <c r="B455" s="1"/>
       <c r="C455" s="2">
         <v>74</v>
@@ -13621,7 +13698,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="456" spans="2:7">
+    <row r="456" spans="1:7">
+      <c r="A456" s="5"/>
       <c r="B456" s="1"/>
       <c r="C456" s="2">
         <v>75</v>
@@ -13639,7 +13717,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="457" spans="2:7">
+    <row r="457" spans="1:7">
+      <c r="A457" s="5"/>
       <c r="B457" s="1" t="s">
         <v>30</v>
       </c>
@@ -13659,7 +13738,8 @@
         <v>29</v>
       </c>
     </row>
-    <row r="458" spans="2:7">
+    <row r="458" spans="1:7">
+      <c r="A458" s="5"/>
       <c r="B458" s="1"/>
       <c r="C458" s="2">
         <v>1</v>
@@ -13677,7 +13757,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="459" spans="2:7">
+    <row r="459" spans="1:7">
+      <c r="A459" s="5"/>
       <c r="B459" s="1"/>
       <c r="C459" s="2">
         <v>2</v>
@@ -13695,7 +13776,8 @@
         <v>0.714285714285714</v>
       </c>
     </row>
-    <row r="460" spans="2:7">
+    <row r="460" spans="1:7">
+      <c r="A460" s="5"/>
       <c r="B460" s="1"/>
       <c r="C460" s="2">
         <v>3</v>
@@ -13713,7 +13795,8 @@
         <v>0.785714285714286</v>
       </c>
     </row>
-    <row r="461" spans="2:7">
+    <row r="461" spans="1:7">
+      <c r="A461" s="5"/>
       <c r="B461" s="1"/>
       <c r="C461" s="2">
         <v>4</v>
@@ -13731,7 +13814,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="462" spans="2:7">
+    <row r="462" spans="1:7">
+      <c r="A462" s="5"/>
       <c r="B462" s="1"/>
       <c r="C462" s="2">
         <v>5</v>
@@ -13749,7 +13833,8 @@
         <v>0.642857142857143</v>
       </c>
     </row>
-    <row r="463" spans="2:7">
+    <row r="463" spans="1:7">
+      <c r="A463" s="5"/>
       <c r="B463" s="1"/>
       <c r="C463" s="2">
         <v>6</v>
@@ -13767,7 +13852,8 @@
         <v>0.785714285714286</v>
       </c>
     </row>
-    <row r="464" spans="2:7">
+    <row r="464" spans="1:7">
+      <c r="A464" s="5"/>
       <c r="B464" s="1"/>
       <c r="C464" s="2">
         <v>7</v>
@@ -13785,7 +13871,8 @@
         <v>0.642857142857143</v>
       </c>
     </row>
-    <row r="465" spans="2:7">
+    <row r="465" spans="1:7">
+      <c r="A465" s="5"/>
       <c r="B465" s="1"/>
       <c r="C465" s="2">
         <v>8</v>
@@ -13803,7 +13890,8 @@
         <v>0.785714285714286</v>
       </c>
     </row>
-    <row r="466" spans="2:7">
+    <row r="466" spans="1:7">
+      <c r="A466" s="5"/>
       <c r="B466" s="1"/>
       <c r="C466" s="2">
         <v>9</v>
@@ -13821,7 +13909,8 @@
         <v>0.714285714285714</v>
       </c>
     </row>
-    <row r="467" spans="2:7">
+    <row r="467" spans="1:7">
+      <c r="A467" s="5"/>
       <c r="B467" s="1"/>
       <c r="C467" s="2">
         <v>10</v>
@@ -13839,7 +13928,8 @@
         <v>0.785714285714286</v>
       </c>
     </row>
-    <row r="468" spans="2:7">
+    <row r="468" spans="1:7">
+      <c r="A468" s="5"/>
       <c r="B468" s="1"/>
       <c r="C468" s="2">
         <v>11</v>
@@ -13857,7 +13947,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="469" spans="2:7">
+    <row r="469" spans="1:7">
+      <c r="A469" s="5"/>
       <c r="B469" s="1"/>
       <c r="C469" s="2">
         <v>12</v>
@@ -13875,7 +13966,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="470" spans="2:7">
+    <row r="470" spans="1:7">
+      <c r="A470" s="5"/>
       <c r="B470" s="1"/>
       <c r="C470" s="2">
         <v>13</v>
@@ -13893,7 +13985,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="471" spans="2:7">
+    <row r="471" spans="1:7">
+      <c r="A471" s="5"/>
       <c r="B471" s="1"/>
       <c r="C471" s="2">
         <v>14</v>
@@ -13911,7 +14004,8 @@
         <v>0.785714285714286</v>
       </c>
     </row>
-    <row r="472" spans="2:7">
+    <row r="472" spans="1:7">
+      <c r="A472" s="5"/>
       <c r="B472" s="1"/>
       <c r="C472" s="2">
         <v>15</v>
@@ -13929,7 +14023,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="473" spans="2:7">
+    <row r="473" spans="1:7">
+      <c r="A473" s="5"/>
       <c r="B473" s="1"/>
       <c r="C473" s="2">
         <v>16</v>
@@ -13947,7 +14042,8 @@
         <v>0.571428571428571</v>
       </c>
     </row>
-    <row r="474" spans="2:7">
+    <row r="474" spans="1:7">
+      <c r="A474" s="5"/>
       <c r="B474" s="1"/>
       <c r="C474" s="2">
         <v>17</v>
@@ -13965,7 +14061,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="475" spans="2:7">
+    <row r="475" spans="1:7">
+      <c r="A475" s="5"/>
       <c r="B475" s="1"/>
       <c r="C475" s="2">
         <v>18</v>
@@ -13983,7 +14080,8 @@
         <v>0.714285714285714</v>
       </c>
     </row>
-    <row r="476" spans="2:7">
+    <row r="476" spans="1:7">
+      <c r="A476" s="5"/>
       <c r="B476" s="1"/>
       <c r="C476" s="2">
         <v>19</v>
@@ -14001,7 +14099,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="477" spans="2:7">
+    <row r="477" spans="1:7">
+      <c r="A477" s="5"/>
       <c r="B477" s="1"/>
       <c r="C477" s="2">
         <v>20</v>
@@ -14019,7 +14118,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="478" spans="2:7">
+    <row r="478" spans="1:7">
+      <c r="A478" s="5"/>
       <c r="B478" s="1"/>
       <c r="C478" s="2">
         <v>21</v>
@@ -14037,7 +14137,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="479" spans="2:7">
+    <row r="479" spans="1:7">
+      <c r="A479" s="5"/>
       <c r="B479" s="1"/>
       <c r="C479" s="2">
         <v>22</v>
@@ -14055,7 +14156,8 @@
         <v>0.142857142857143</v>
       </c>
     </row>
-    <row r="480" spans="2:7">
+    <row r="480" spans="1:7">
+      <c r="A480" s="5"/>
       <c r="B480" s="1"/>
       <c r="C480" s="2">
         <v>23</v>
@@ -14073,7 +14175,8 @@
         <v>0.785714285714286</v>
       </c>
     </row>
-    <row r="481" spans="2:7">
+    <row r="481" spans="1:7">
+      <c r="A481" s="5"/>
       <c r="B481" s="1"/>
       <c r="C481" s="2">
         <v>24</v>
@@ -14091,7 +14194,8 @@
         <v>0.785714285714286</v>
       </c>
     </row>
-    <row r="482" spans="2:7">
+    <row r="482" spans="1:7">
+      <c r="A482" s="5"/>
       <c r="B482" s="1"/>
       <c r="C482" s="2">
         <v>25</v>
@@ -14109,7 +14213,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="483" spans="2:7">
+    <row r="483" spans="1:7">
+      <c r="A483" s="5"/>
       <c r="B483" s="1"/>
       <c r="C483" s="2">
         <v>26</v>
@@ -14127,7 +14232,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="484" spans="2:7">
+    <row r="484" spans="1:7">
+      <c r="A484" s="5"/>
       <c r="B484" s="1"/>
       <c r="C484" s="2">
         <v>27</v>
@@ -14145,7 +14251,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="485" spans="2:7">
+    <row r="485" spans="1:7">
+      <c r="A485" s="5"/>
       <c r="B485" s="1"/>
       <c r="C485" s="2">
         <v>28</v>
@@ -14163,7 +14270,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="486" spans="2:7">
+    <row r="486" spans="1:7">
+      <c r="A486" s="5"/>
       <c r="B486" s="1"/>
       <c r="C486" s="2">
         <v>29</v>
@@ -14181,7 +14289,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="487" spans="2:7">
+    <row r="487" spans="1:7">
+      <c r="A487" s="5"/>
       <c r="B487" s="1"/>
       <c r="C487" s="2">
         <v>30</v>
@@ -14199,7 +14308,8 @@
         <v>0.928571428571429</v>
       </c>
     </row>
-    <row r="488" spans="2:7">
+    <row r="488" spans="1:7">
+      <c r="A488" s="5"/>
       <c r="B488" s="1"/>
       <c r="C488" s="2">
         <v>31</v>
@@ -14217,7 +14327,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="489" spans="2:7">
+    <row r="489" spans="1:7">
+      <c r="A489" s="5"/>
       <c r="B489" s="1"/>
       <c r="C489" s="2">
         <v>32</v>
@@ -14235,7 +14346,8 @@
         <v>0.785714285714286</v>
       </c>
     </row>
-    <row r="490" spans="2:7">
+    <row r="490" spans="1:7">
+      <c r="A490" s="5"/>
       <c r="B490" s="1"/>
       <c r="C490" s="2">
         <v>33</v>
@@ -14253,7 +14365,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="491" spans="2:7">
+    <row r="491" spans="1:7">
+      <c r="A491" s="5"/>
       <c r="B491" s="1"/>
       <c r="C491" s="2">
         <v>34</v>
@@ -14271,7 +14384,8 @@
         <v>0.0714285714285714</v>
       </c>
     </row>
-    <row r="492" spans="2:7">
+    <row r="492" spans="1:7">
+      <c r="A492" s="5"/>
       <c r="B492" s="1"/>
       <c r="C492" s="2">
         <v>35</v>
@@ -14289,7 +14403,8 @@
         <v>0.0714285714285714</v>
       </c>
     </row>
-    <row r="493" spans="2:7">
+    <row r="493" spans="1:7">
+      <c r="A493" s="5"/>
       <c r="B493" s="1"/>
       <c r="C493" s="2">
         <v>36</v>
@@ -14307,7 +14422,8 @@
         <v>0.857142857142857</v>
       </c>
     </row>
-    <row r="494" spans="2:7">
+    <row r="494" spans="1:7">
+      <c r="A494" s="5"/>
       <c r="B494" s="1"/>
       <c r="C494" s="2">
         <v>37</v>
@@ -14325,7 +14441,8 @@
         <v>0.214285714285714</v>
       </c>
     </row>
-    <row r="495" spans="2:7">
+    <row r="495" spans="1:7">
+      <c r="A495" s="5"/>
       <c r="B495" s="1"/>
       <c r="C495" s="2">
         <v>38</v>
@@ -14343,7 +14460,8 @@
         <v>0.857142857142857</v>
       </c>
     </row>
-    <row r="496" spans="2:7">
+    <row r="496" spans="1:7">
+      <c r="A496" s="5"/>
       <c r="B496" s="1"/>
       <c r="C496" s="2">
         <v>39</v>
@@ -14361,7 +14479,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="497" spans="2:7">
+    <row r="497" spans="1:7">
+      <c r="A497" s="5"/>
       <c r="B497" s="1"/>
       <c r="C497" s="2">
         <v>40</v>
@@ -14379,7 +14498,8 @@
         <v>0.857142857142857</v>
       </c>
     </row>
-    <row r="498" spans="2:7">
+    <row r="498" spans="1:7">
+      <c r="A498" s="5"/>
       <c r="B498" s="1"/>
       <c r="C498" s="2">
         <v>41</v>
@@ -14397,7 +14517,8 @@
         <v>0.928571428571429</v>
       </c>
     </row>
-    <row r="499" spans="2:7">
+    <row r="499" spans="1:7">
+      <c r="A499" s="5"/>
       <c r="B499" s="1"/>
       <c r="C499" s="2">
         <v>42</v>
@@ -14415,7 +14536,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="500" spans="2:7">
+    <row r="500" spans="1:7">
+      <c r="A500" s="5"/>
       <c r="B500" s="1"/>
       <c r="C500" s="2">
         <v>43</v>
@@ -14433,7 +14555,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="501" spans="2:7">
+    <row r="501" spans="1:7">
+      <c r="A501" s="5"/>
       <c r="B501" s="1"/>
       <c r="C501" s="2">
         <v>44</v>
@@ -14451,7 +14574,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="502" spans="2:7">
+    <row r="502" spans="1:7">
+      <c r="A502" s="5"/>
       <c r="B502" s="1"/>
       <c r="C502" s="2">
         <v>45</v>
@@ -14469,7 +14593,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="503" spans="2:7">
+    <row r="503" spans="1:7">
+      <c r="A503" s="5"/>
       <c r="B503" s="1"/>
       <c r="C503" s="2">
         <v>46</v>
@@ -14487,7 +14612,8 @@
         <v>0.857142857142857</v>
       </c>
     </row>
-    <row r="504" spans="2:7">
+    <row r="504" spans="1:7">
+      <c r="A504" s="5"/>
       <c r="B504" s="1"/>
       <c r="C504" s="2">
         <v>47</v>
@@ -14505,7 +14631,8 @@
         <v>0.0714285714285714</v>
       </c>
     </row>
-    <row r="505" spans="2:7">
+    <row r="505" spans="1:7">
+      <c r="A505" s="5"/>
       <c r="B505" s="1"/>
       <c r="C505" s="2">
         <v>48</v>
@@ -14523,7 +14650,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="506" spans="2:7">
+    <row r="506" spans="1:7">
+      <c r="A506" s="5"/>
       <c r="B506" s="1"/>
       <c r="C506" s="2">
         <v>49</v>
@@ -14541,7 +14669,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="507" spans="2:7">
+    <row r="507" spans="1:7">
+      <c r="A507" s="5"/>
       <c r="B507" s="1"/>
       <c r="C507" s="2">
         <v>50</v>
@@ -14559,7 +14688,8 @@
         <v>0.928571428571429</v>
       </c>
     </row>
-    <row r="508" spans="2:7">
+    <row r="508" spans="1:7">
+      <c r="A508" s="5"/>
       <c r="B508" s="1"/>
       <c r="C508" s="2">
         <v>51</v>
@@ -14577,7 +14707,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="509" spans="2:7">
+    <row r="509" spans="1:7">
+      <c r="A509" s="5"/>
       <c r="B509" s="1"/>
       <c r="C509" s="2">
         <v>52</v>
@@ -14595,7 +14726,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="510" spans="2:7">
+    <row r="510" spans="1:7">
+      <c r="A510" s="5"/>
       <c r="B510" s="1"/>
       <c r="C510" s="2">
         <v>53</v>
@@ -14613,7 +14745,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="511" spans="2:7">
+    <row r="511" spans="1:7">
+      <c r="A511" s="5"/>
       <c r="B511" s="1"/>
       <c r="C511" s="2">
         <v>54</v>
@@ -14631,7 +14764,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="512" spans="2:7">
+    <row r="512" spans="1:7">
+      <c r="A512" s="5"/>
       <c r="B512" s="1"/>
       <c r="C512" s="2">
         <v>55</v>
@@ -14649,7 +14783,8 @@
         <v>0.928571428571429</v>
       </c>
     </row>
-    <row r="513" spans="2:7">
+    <row r="513" spans="1:7">
+      <c r="A513" s="5"/>
       <c r="B513" s="1"/>
       <c r="C513" s="2">
         <v>56</v>
@@ -14667,7 +14802,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="514" spans="2:7">
+    <row r="514" spans="1:7">
+      <c r="A514" s="5"/>
       <c r="B514" s="1"/>
       <c r="C514" s="2">
         <v>57</v>
@@ -14685,7 +14821,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="515" spans="2:7">
+    <row r="515" spans="1:7">
+      <c r="A515" s="5"/>
       <c r="B515" s="1"/>
       <c r="C515" s="2">
         <v>58</v>
@@ -14703,7 +14840,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="516" spans="2:7">
+    <row r="516" spans="1:7">
+      <c r="A516" s="5"/>
       <c r="B516" s="1"/>
       <c r="C516" s="2">
         <v>59</v>
@@ -14721,7 +14859,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="517" spans="2:7">
+    <row r="517" spans="1:7">
+      <c r="A517" s="5"/>
       <c r="B517" s="1"/>
       <c r="C517" s="2">
         <v>60</v>
@@ -14739,7 +14878,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="518" spans="2:7">
+    <row r="518" spans="1:7">
+      <c r="A518" s="5"/>
       <c r="B518" s="1"/>
       <c r="C518" s="2">
         <v>61</v>
@@ -14757,7 +14897,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="519" spans="2:7">
+    <row r="519" spans="1:7">
+      <c r="A519" s="5"/>
       <c r="B519" s="1"/>
       <c r="C519" s="2">
         <v>62</v>
@@ -14775,7 +14916,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="520" spans="2:7">
+    <row r="520" spans="1:7">
+      <c r="A520" s="5"/>
       <c r="B520" s="1"/>
       <c r="C520" s="2">
         <v>63</v>
@@ -14793,7 +14935,8 @@
         <v>0.928571428571429</v>
       </c>
     </row>
-    <row r="521" spans="2:7">
+    <row r="521" spans="1:7">
+      <c r="A521" s="5"/>
       <c r="B521" s="1"/>
       <c r="C521" s="2">
         <v>64</v>
@@ -14811,7 +14954,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="522" spans="2:7">
+    <row r="522" spans="1:7">
+      <c r="A522" s="5"/>
       <c r="B522" s="1"/>
       <c r="C522" s="2">
         <v>65</v>
@@ -14829,7 +14973,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="523" spans="2:7">
+    <row r="523" spans="1:7">
+      <c r="A523" s="5"/>
       <c r="B523" s="1"/>
       <c r="C523" s="2">
         <v>66</v>
@@ -14847,7 +14992,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="524" spans="2:7">
+    <row r="524" spans="1:7">
+      <c r="A524" s="5"/>
       <c r="B524" s="1"/>
       <c r="C524" s="2">
         <v>67</v>
@@ -14865,7 +15011,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="525" spans="2:7">
+    <row r="525" spans="1:7">
+      <c r="A525" s="5"/>
       <c r="B525" s="1"/>
       <c r="C525" s="2">
         <v>68</v>
@@ -14883,7 +15030,8 @@
         <v>0.0714285714285714</v>
       </c>
     </row>
-    <row r="526" spans="2:7">
+    <row r="526" spans="1:7">
+      <c r="A526" s="5"/>
       <c r="B526" s="1"/>
       <c r="C526" s="2">
         <v>69</v>
@@ -14901,7 +15049,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="527" spans="2:7">
+    <row r="527" spans="1:7">
+      <c r="A527" s="5"/>
       <c r="B527" s="1"/>
       <c r="C527" s="2">
         <v>70</v>
@@ -14919,7 +15068,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="528" spans="2:7">
+    <row r="528" spans="1:7">
+      <c r="A528" s="5"/>
       <c r="B528" s="1"/>
       <c r="C528" s="2">
         <v>71</v>
@@ -14937,7 +15087,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="529" spans="2:7">
+    <row r="529" spans="1:7">
+      <c r="A529" s="5"/>
       <c r="B529" s="1"/>
       <c r="C529" s="2">
         <v>72</v>
@@ -14955,7 +15106,8 @@
         <v>0.928571428571429</v>
       </c>
     </row>
-    <row r="530" spans="2:7">
+    <row r="530" spans="1:7">
+      <c r="A530" s="5"/>
       <c r="B530" s="1"/>
       <c r="C530" s="2">
         <v>73</v>
@@ -14973,7 +15125,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="531" spans="2:7">
+    <row r="531" spans="1:7">
+      <c r="A531" s="5"/>
       <c r="B531" s="1"/>
       <c r="C531" s="2">
         <v>74</v>
@@ -14991,7 +15144,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="532" spans="2:7">
+    <row r="532" spans="1:7">
+      <c r="A532" s="5"/>
       <c r="B532" s="1"/>
       <c r="C532" s="2">
         <v>75</v>
@@ -15009,7 +15163,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="533" spans="2:7">
+    <row r="533" spans="1:7">
+      <c r="A533" s="5"/>
       <c r="B533" s="1" t="s">
         <v>31</v>
       </c>
@@ -15029,7 +15184,8 @@
         <v>29</v>
       </c>
     </row>
-    <row r="534" spans="2:7">
+    <row r="534" spans="1:7">
+      <c r="A534" s="5"/>
       <c r="B534" s="1"/>
       <c r="C534" s="2">
         <v>1</v>
@@ -15047,7 +15203,8 @@
         <v>0.928571428571429</v>
       </c>
     </row>
-    <row r="535" spans="2:7">
+    <row r="535" spans="1:7">
+      <c r="A535" s="5"/>
       <c r="B535" s="1"/>
       <c r="C535" s="2">
         <v>2</v>
@@ -15065,7 +15222,8 @@
         <v>0.928571428571429</v>
       </c>
     </row>
-    <row r="536" spans="2:7">
+    <row r="536" spans="1:7">
+      <c r="A536" s="5"/>
       <c r="B536" s="1"/>
       <c r="C536" s="2">
         <v>3</v>
@@ -15083,7 +15241,8 @@
         <v>0.928571428571429</v>
       </c>
     </row>
-    <row r="537" spans="2:7">
+    <row r="537" spans="1:7">
+      <c r="A537" s="5"/>
       <c r="B537" s="1"/>
       <c r="C537" s="2">
         <v>4</v>
@@ -15101,7 +15260,8 @@
         <v>0.857142857142857</v>
       </c>
     </row>
-    <row r="538" spans="2:7">
+    <row r="538" spans="1:7">
+      <c r="A538" s="5"/>
       <c r="B538" s="1"/>
       <c r="C538" s="2">
         <v>5</v>
@@ -15119,7 +15279,8 @@
         <v>0.571428571428571</v>
       </c>
     </row>
-    <row r="539" spans="2:7">
+    <row r="539" spans="1:7">
+      <c r="A539" s="5"/>
       <c r="B539" s="1"/>
       <c r="C539" s="2">
         <v>6</v>
@@ -15137,7 +15298,8 @@
         <v>0.928571428571429</v>
       </c>
     </row>
-    <row r="540" spans="2:7">
+    <row r="540" spans="1:7">
+      <c r="A540" s="5"/>
       <c r="B540" s="1"/>
       <c r="C540" s="2">
         <v>7</v>
@@ -15155,7 +15317,8 @@
         <v>0.714285714285714</v>
       </c>
     </row>
-    <row r="541" spans="2:7">
+    <row r="541" spans="1:7">
+      <c r="A541" s="5"/>
       <c r="B541" s="1"/>
       <c r="C541" s="2">
         <v>8</v>
@@ -15173,7 +15336,8 @@
         <v>0.928571428571429</v>
       </c>
     </row>
-    <row r="542" spans="2:7">
+    <row r="542" spans="1:7">
+      <c r="A542" s="5"/>
       <c r="B542" s="1"/>
       <c r="C542" s="2">
         <v>9</v>
@@ -15191,7 +15355,8 @@
         <v>0.785714285714286</v>
       </c>
     </row>
-    <row r="543" spans="2:7">
+    <row r="543" spans="1:7">
+      <c r="A543" s="5"/>
       <c r="B543" s="1"/>
       <c r="C543" s="2">
         <v>10</v>
@@ -15209,7 +15374,8 @@
         <v>0.785714285714286</v>
       </c>
     </row>
-    <row r="544" spans="2:7">
+    <row r="544" spans="1:7">
+      <c r="A544" s="5"/>
       <c r="B544" s="1"/>
       <c r="C544" s="2">
         <v>11</v>
@@ -15227,7 +15393,8 @@
         <v>0.928571428571429</v>
       </c>
     </row>
-    <row r="545" spans="2:7">
+    <row r="545" spans="1:7">
+      <c r="A545" s="5"/>
       <c r="B545" s="1"/>
       <c r="C545" s="2">
         <v>12</v>
@@ -15245,7 +15412,8 @@
         <v>0.928571428571429</v>
       </c>
     </row>
-    <row r="546" spans="2:7">
+    <row r="546" spans="1:7">
+      <c r="A546" s="5"/>
       <c r="B546" s="1"/>
       <c r="C546" s="2">
         <v>13</v>
@@ -15263,7 +15431,8 @@
         <v>0.785714285714286</v>
       </c>
     </row>
-    <row r="547" spans="2:7">
+    <row r="547" spans="1:7">
+      <c r="A547" s="5"/>
       <c r="B547" s="1"/>
       <c r="C547" s="2">
         <v>14</v>
@@ -15281,7 +15450,8 @@
         <v>0.785714285714286</v>
       </c>
     </row>
-    <row r="548" spans="2:7">
+    <row r="548" spans="1:7">
+      <c r="A548" s="5"/>
       <c r="B548" s="1"/>
       <c r="C548" s="2">
         <v>15</v>
@@ -15299,7 +15469,8 @@
         <v>0.928571428571429</v>
       </c>
     </row>
-    <row r="549" spans="2:7">
+    <row r="549" spans="1:7">
+      <c r="A549" s="5"/>
       <c r="B549" s="1"/>
       <c r="C549" s="2">
         <v>16</v>
@@ -15317,7 +15488,8 @@
         <v>0.928571428571429</v>
       </c>
     </row>
-    <row r="550" spans="2:7">
+    <row r="550" spans="1:7">
+      <c r="A550" s="5"/>
       <c r="B550" s="1"/>
       <c r="C550" s="2">
         <v>17</v>
@@ -15335,7 +15507,8 @@
         <v>0.928571428571429</v>
       </c>
     </row>
-    <row r="551" spans="2:7">
+    <row r="551" spans="1:7">
+      <c r="A551" s="5"/>
       <c r="B551" s="1"/>
       <c r="C551" s="2">
         <v>18</v>
@@ -15353,7 +15526,8 @@
         <v>0.357142857142857</v>
       </c>
     </row>
-    <row r="552" spans="2:7">
+    <row r="552" spans="1:7">
+      <c r="A552" s="5"/>
       <c r="B552" s="1"/>
       <c r="C552" s="2">
         <v>19</v>
@@ -15371,7 +15545,8 @@
         <v>0.928571428571429</v>
       </c>
     </row>
-    <row r="553" spans="2:7">
+    <row r="553" spans="1:7">
+      <c r="A553" s="5"/>
       <c r="B553" s="1"/>
       <c r="C553" s="2">
         <v>20</v>
@@ -15389,7 +15564,8 @@
         <v>0.714285714285714</v>
       </c>
     </row>
-    <row r="554" spans="2:7">
+    <row r="554" spans="1:7">
+      <c r="A554" s="5"/>
       <c r="B554" s="1"/>
       <c r="C554" s="2">
         <v>21</v>
@@ -15407,7 +15583,8 @@
         <v>0.785714285714286</v>
       </c>
     </row>
-    <row r="555" spans="2:7">
+    <row r="555" spans="1:7">
+      <c r="A555" s="5"/>
       <c r="B555" s="1"/>
       <c r="C555" s="2">
         <v>22</v>
@@ -15425,7 +15602,8 @@
         <v>0.857142857142857</v>
       </c>
     </row>
-    <row r="556" spans="2:7">
+    <row r="556" spans="1:7">
+      <c r="A556" s="5"/>
       <c r="B556" s="1"/>
       <c r="C556" s="2">
         <v>23</v>
@@ -15443,7 +15621,8 @@
         <v>0.785714285714286</v>
       </c>
     </row>
-    <row r="557" spans="2:7">
+    <row r="557" spans="1:7">
+      <c r="A557" s="5"/>
       <c r="B557" s="1"/>
       <c r="C557" s="2">
         <v>24</v>
@@ -15461,7 +15640,8 @@
         <v>0.785714285714286</v>
       </c>
     </row>
-    <row r="558" spans="2:7">
+    <row r="558" spans="1:7">
+      <c r="A558" s="5"/>
       <c r="B558" s="1"/>
       <c r="C558" s="2">
         <v>25</v>
@@ -15479,7 +15659,8 @@
         <v>0.928571428571429</v>
       </c>
     </row>
-    <row r="559" spans="2:7">
+    <row r="559" spans="1:7">
+      <c r="A559" s="5"/>
       <c r="B559" s="1"/>
       <c r="C559" s="2">
         <v>26</v>
@@ -15497,7 +15678,8 @@
         <v>0.785714285714286</v>
       </c>
     </row>
-    <row r="560" spans="2:7">
+    <row r="560" spans="1:7">
+      <c r="A560" s="5"/>
       <c r="B560" s="1"/>
       <c r="C560" s="2">
         <v>27</v>
@@ -15515,7 +15697,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="561" spans="2:7">
+    <row r="561" spans="1:7">
+      <c r="A561" s="5"/>
       <c r="B561" s="1"/>
       <c r="C561" s="2">
         <v>28</v>
@@ -15533,7 +15716,8 @@
         <v>0.785714285714286</v>
       </c>
     </row>
-    <row r="562" spans="2:7">
+    <row r="562" spans="1:7">
+      <c r="A562" s="5"/>
       <c r="B562" s="1"/>
       <c r="C562" s="2">
         <v>29</v>
@@ -15551,7 +15735,8 @@
         <v>0.642857142857143</v>
       </c>
     </row>
-    <row r="563" spans="2:7">
+    <row r="563" spans="1:7">
+      <c r="A563" s="5"/>
       <c r="B563" s="1"/>
       <c r="C563" s="2">
         <v>30</v>
@@ -15569,7 +15754,8 @@
         <v>0.785714285714286</v>
       </c>
     </row>
-    <row r="564" spans="2:7">
+    <row r="564" spans="1:7">
+      <c r="A564" s="5"/>
       <c r="B564" s="1"/>
       <c r="C564" s="2">
         <v>31</v>
@@ -15587,7 +15773,8 @@
         <v>0.642857142857143</v>
       </c>
     </row>
-    <row r="565" spans="2:7">
+    <row r="565" spans="1:7">
+      <c r="A565" s="5"/>
       <c r="B565" s="1"/>
       <c r="C565" s="2">
         <v>32</v>
@@ -15605,7 +15792,8 @@
         <v>0.928571428571429</v>
       </c>
     </row>
-    <row r="566" spans="2:7">
+    <row r="566" spans="1:7">
+      <c r="A566" s="5"/>
       <c r="B566" s="1"/>
       <c r="C566" s="2">
         <v>33</v>
@@ -15623,7 +15811,8 @@
         <v>0.928571428571429</v>
       </c>
     </row>
-    <row r="567" spans="2:7">
+    <row r="567" spans="1:7">
+      <c r="A567" s="5"/>
       <c r="B567" s="1"/>
       <c r="C567" s="2">
         <v>34</v>
@@ -15641,7 +15830,8 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="568" spans="2:7">
+    <row r="568" spans="1:7">
+      <c r="A568" s="5"/>
       <c r="B568" s="1"/>
       <c r="C568" s="2">
         <v>35</v>
@@ -15659,7 +15849,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="569" spans="2:7">
+    <row r="569" spans="1:7">
+      <c r="A569" s="5"/>
       <c r="B569" s="1"/>
       <c r="C569" s="2">
         <v>36</v>
@@ -15677,7 +15868,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="570" spans="2:7">
+    <row r="570" spans="1:7">
+      <c r="A570" s="5"/>
       <c r="B570" s="1"/>
       <c r="C570" s="2">
         <v>37</v>
@@ -15695,7 +15887,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="571" spans="2:7">
+    <row r="571" spans="1:7">
+      <c r="A571" s="5"/>
       <c r="B571" s="1"/>
       <c r="C571" s="2">
         <v>38</v>
@@ -15713,7 +15906,8 @@
         <v>0.857142857142857</v>
       </c>
     </row>
-    <row r="572" spans="2:7">
+    <row r="572" spans="1:7">
+      <c r="A572" s="5"/>
       <c r="B572" s="1"/>
       <c r="C572" s="2">
         <v>39</v>
@@ -15731,7 +15925,8 @@
         <v>0.857142857142857</v>
       </c>
     </row>
-    <row r="573" spans="2:7">
+    <row r="573" spans="1:7">
+      <c r="A573" s="5"/>
       <c r="B573" s="1"/>
       <c r="C573" s="2">
         <v>40</v>
@@ -15749,7 +15944,8 @@
         <v>0.785714285714286</v>
       </c>
     </row>
-    <row r="574" spans="2:7">
+    <row r="574" spans="1:7">
+      <c r="A574" s="5"/>
       <c r="B574" s="1"/>
       <c r="C574" s="2">
         <v>41</v>
@@ -15767,7 +15963,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="575" spans="2:7">
+    <row r="575" spans="1:7">
+      <c r="A575" s="5"/>
       <c r="B575" s="1"/>
       <c r="C575" s="2">
         <v>42</v>
@@ -15785,7 +15982,8 @@
         <v>0.857142857142857</v>
       </c>
     </row>
-    <row r="576" spans="2:7">
+    <row r="576" spans="1:7">
+      <c r="A576" s="5"/>
       <c r="B576" s="1"/>
       <c r="C576" s="2">
         <v>43</v>
@@ -15803,7 +16001,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="577" spans="2:7">
+    <row r="577" spans="1:7">
+      <c r="A577" s="5"/>
       <c r="B577" s="1"/>
       <c r="C577" s="2">
         <v>44</v>
@@ -15821,7 +16020,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="578" spans="2:7">
+    <row r="578" spans="1:7">
+      <c r="A578" s="5"/>
       <c r="B578" s="1"/>
       <c r="C578" s="2">
         <v>45</v>
@@ -15839,7 +16039,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="579" spans="2:7">
+    <row r="579" spans="1:7">
+      <c r="A579" s="5"/>
       <c r="B579" s="1"/>
       <c r="C579" s="2">
         <v>46</v>
@@ -15857,7 +16058,8 @@
         <v>0.857142857142857</v>
       </c>
     </row>
-    <row r="580" spans="2:7">
+    <row r="580" spans="1:7">
+      <c r="A580" s="5"/>
       <c r="B580" s="1"/>
       <c r="C580" s="2">
         <v>47</v>
@@ -15875,7 +16077,8 @@
         <v>0.857142857142857</v>
       </c>
     </row>
-    <row r="581" spans="2:7">
+    <row r="581" spans="1:7">
+      <c r="A581" s="5"/>
       <c r="B581" s="1"/>
       <c r="C581" s="2">
         <v>48</v>
@@ -15893,7 +16096,8 @@
         <v>0.928571428571429</v>
       </c>
     </row>
-    <row r="582" spans="2:7">
+    <row r="582" spans="1:7">
+      <c r="A582" s="5"/>
       <c r="B582" s="1"/>
       <c r="C582" s="2">
         <v>49</v>
@@ -15911,7 +16115,8 @@
         <v>0.928571428571429</v>
       </c>
     </row>
-    <row r="583" spans="2:7">
+    <row r="583" spans="1:7">
+      <c r="A583" s="5"/>
       <c r="B583" s="1"/>
       <c r="C583" s="2">
         <v>50</v>
@@ -15929,7 +16134,8 @@
         <v>0.857142857142857</v>
       </c>
     </row>
-    <row r="584" spans="2:7">
+    <row r="584" spans="1:7">
+      <c r="A584" s="5"/>
       <c r="B584" s="1"/>
       <c r="C584" s="2">
         <v>51</v>
@@ -15947,7 +16153,8 @@
         <v>0.928571428571429</v>
       </c>
     </row>
-    <row r="585" spans="2:7">
+    <row r="585" spans="1:7">
+      <c r="A585" s="5"/>
       <c r="B585" s="1"/>
       <c r="C585" s="2">
         <v>52</v>
@@ -15965,7 +16172,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="586" spans="2:7">
+    <row r="586" spans="1:7">
+      <c r="A586" s="5"/>
       <c r="B586" s="1"/>
       <c r="C586" s="2">
         <v>53</v>
@@ -15983,7 +16191,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="587" spans="2:7">
+    <row r="587" spans="1:7">
+      <c r="A587" s="5"/>
       <c r="B587" s="1"/>
       <c r="C587" s="2">
         <v>54</v>
@@ -16001,7 +16210,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="588" spans="2:7">
+    <row r="588" spans="1:7">
+      <c r="A588" s="5"/>
       <c r="B588" s="1"/>
       <c r="C588" s="2">
         <v>55</v>
@@ -16019,7 +16229,8 @@
         <v>0.928571428571429</v>
       </c>
     </row>
-    <row r="589" spans="2:7">
+    <row r="589" spans="1:7">
+      <c r="A589" s="5"/>
       <c r="B589" s="1"/>
       <c r="C589" s="2">
         <v>56</v>
@@ -16037,7 +16248,8 @@
         <v>0.928571428571429</v>
       </c>
     </row>
-    <row r="590" spans="2:7">
+    <row r="590" spans="1:7">
+      <c r="A590" s="5"/>
       <c r="B590" s="1"/>
       <c r="C590" s="2">
         <v>57</v>
@@ -16055,7 +16267,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="591" spans="2:7">
+    <row r="591" spans="1:7">
+      <c r="A591" s="5"/>
       <c r="B591" s="1"/>
       <c r="C591" s="2">
         <v>58</v>
@@ -16073,7 +16286,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="592" spans="2:7">
+    <row r="592" spans="1:7">
+      <c r="A592" s="5"/>
       <c r="B592" s="1"/>
       <c r="C592" s="2">
         <v>59</v>
@@ -16091,7 +16305,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="593" spans="2:7">
+    <row r="593" spans="1:7">
+      <c r="A593" s="5"/>
       <c r="B593" s="1"/>
       <c r="C593" s="2">
         <v>60</v>
@@ -16109,7 +16324,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="594" spans="2:7">
+    <row r="594" spans="1:7">
+      <c r="A594" s="5"/>
       <c r="B594" s="1"/>
       <c r="C594" s="2">
         <v>61</v>
@@ -16127,7 +16343,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="595" spans="2:7">
+    <row r="595" spans="1:7">
+      <c r="A595" s="5"/>
       <c r="B595" s="1"/>
       <c r="C595" s="2">
         <v>62</v>
@@ -16145,7 +16362,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="596" spans="2:7">
+    <row r="596" spans="1:7">
+      <c r="A596" s="5"/>
       <c r="B596" s="1"/>
       <c r="C596" s="2">
         <v>63</v>
@@ -16163,7 +16381,8 @@
         <v>0.928571428571429</v>
       </c>
     </row>
-    <row r="597" spans="2:7">
+    <row r="597" spans="1:7">
+      <c r="A597" s="5"/>
       <c r="B597" s="1"/>
       <c r="C597" s="2">
         <v>64</v>
@@ -16181,7 +16400,8 @@
         <v>0.785714285714286</v>
       </c>
     </row>
-    <row r="598" spans="2:7">
+    <row r="598" spans="1:7">
+      <c r="A598" s="5"/>
       <c r="B598" s="1"/>
       <c r="C598" s="2">
         <v>65</v>
@@ -16199,7 +16419,8 @@
         <v>0.642857142857143</v>
       </c>
     </row>
-    <row r="599" spans="2:7">
+    <row r="599" spans="1:7">
+      <c r="A599" s="5"/>
       <c r="B599" s="1"/>
       <c r="C599" s="2">
         <v>66</v>
@@ -16217,7 +16438,8 @@
         <v>0.928571428571429</v>
       </c>
     </row>
-    <row r="600" spans="2:7">
+    <row r="600" spans="1:7">
+      <c r="A600" s="5"/>
       <c r="B600" s="1"/>
       <c r="C600" s="2">
         <v>67</v>
@@ -16235,7 +16457,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="601" spans="2:7">
+    <row r="601" spans="1:7">
+      <c r="A601" s="5"/>
       <c r="B601" s="1"/>
       <c r="C601" s="2">
         <v>68</v>
@@ -16253,7 +16476,8 @@
         <v>0.928571428571429</v>
       </c>
     </row>
-    <row r="602" spans="2:7">
+    <row r="602" spans="1:7">
+      <c r="A602" s="5"/>
       <c r="B602" s="1"/>
       <c r="C602" s="2">
         <v>69</v>
@@ -16271,7 +16495,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="603" spans="2:7">
+    <row r="603" spans="1:7">
+      <c r="A603" s="5"/>
       <c r="B603" s="1"/>
       <c r="C603" s="2">
         <v>70</v>
@@ -16289,7 +16514,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="604" spans="2:7">
+    <row r="604" spans="1:7">
+      <c r="A604" s="5"/>
       <c r="B604" s="1"/>
       <c r="C604" s="2">
         <v>71</v>
@@ -16307,7 +16533,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="605" spans="2:7">
+    <row r="605" spans="1:7">
+      <c r="A605" s="5"/>
       <c r="B605" s="1"/>
       <c r="C605" s="2">
         <v>72</v>
@@ -16325,7 +16552,8 @@
         <v>0.928571428571429</v>
       </c>
     </row>
-    <row r="606" spans="2:7">
+    <row r="606" spans="1:7">
+      <c r="A606" s="5"/>
       <c r="B606" s="1"/>
       <c r="C606" s="2">
         <v>73</v>
@@ -16343,7 +16571,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="607" spans="2:7">
+    <row r="607" spans="1:7">
+      <c r="A607" s="5"/>
       <c r="B607" s="1"/>
       <c r="C607" s="2">
         <v>74</v>
@@ -16361,7 +16590,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="608" spans="2:7">
+    <row r="608" spans="1:7">
+      <c r="A608" s="5"/>
       <c r="B608" s="1"/>
       <c r="C608" s="2">
         <v>75</v>
@@ -16380,8 +16610,9 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="11">
     <mergeCell ref="A1:A380"/>
+    <mergeCell ref="A381:A608"/>
     <mergeCell ref="B1:B76"/>
     <mergeCell ref="B77:B152"/>
     <mergeCell ref="B153:B228"/>

</xml_diff>